<commit_message>
import functions for pointsourceactivities
</commit_message>
<xml_diff>
--- a/tests/edb/data/pointsourceactivities.xlsx
+++ b/tests/edb/data/pointsourceactivities.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PointSource" sheetId="1" state="visible" r:id="rId2"/>
@@ -211,7 +211,7 @@
     <t xml:space="preserve">g/m3</t>
   </si>
   <si>
-    <t xml:space="preserve">ID </t>
+    <t xml:space="preserve">ID</t>
   </si>
   <si>
     <t xml:space="preserve">typeday</t>
@@ -533,11 +533,11 @@
   </sheetPr>
   <dimension ref="A1:Y8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="10.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="34.18"/>
@@ -919,7 +919,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.73"/>
   </cols>
@@ -971,7 +971,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.98"/>
@@ -1087,11 +1087,11 @@
   </sheetPr>
   <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">

</xml_diff>

<commit_message>
rebase, fix unique constraints and test
</commit_message>
<xml_diff>
--- a/tests/edb/data/pointsourceactivities.xlsx
+++ b/tests/edb/data/pointsourceactivities.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="PointSource" sheetId="1" state="visible" r:id="rId2"/>
@@ -43,10 +43,10 @@
     <t xml:space="preserve">timevar</t>
   </si>
   <si>
-    <t xml:space="preserve">activitycode1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">activitycode2</t>
+    <t xml:space="preserve">activitycode_code_set1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activitycode_code_set2</t>
   </si>
   <si>
     <t xml:space="preserve">activitycode3</t>
@@ -533,11 +533,11 @@
   </sheetPr>
   <dimension ref="A1:Y8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="10.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="34.18"/>
@@ -919,7 +919,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.73"/>
   </cols>
@@ -971,7 +971,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.98"/>
@@ -1087,11 +1087,11 @@
   </sheetPr>
   <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">

</xml_diff>

<commit_message>
fix command import all sheets and fix sheets lost in rebase from tests/edb/data/ xlsx
</commit_message>
<xml_diff>
--- a/tests/edb/data/pointsourceactivities.xlsx
+++ b/tests/edb/data/pointsourceactivities.xlsx
@@ -5,13 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="PointSource" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Activity" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="EmissionFactor" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Timevar" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="CodeSet" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="ActivityCode" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="123">
   <si>
     <t xml:space="preserve">facility_id</t>
   </si>
@@ -350,14 +352,57 @@
   </si>
   <si>
     <t xml:space="preserve">December</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code set 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">code_set1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code set 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">code_set2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">codeset_slug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activitycode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vertical_distribution_slug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PublicPower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Industry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combustion in the production and transformation of energy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -437,7 +482,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -451,6 +496,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -533,11 +582,11 @@
   </sheetPr>
   <dimension ref="A1:Y8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="10.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="34.18"/>
@@ -919,7 +968,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.73"/>
   </cols>
@@ -971,7 +1020,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.98"/>
@@ -1091,7 +1140,7 @@
       <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
@@ -2562,6 +2611,140 @@
       <c r="N54" s="0" t="n">
         <v>100</v>
       </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.17"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="48.62"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
require units to be in file to be imported, not specified generally to function
</commit_message>
<xml_diff>
--- a/tests/edb/data/pointsourceactivities.xlsx
+++ b/tests/edb/data/pointsourceactivities.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="PointSource" sheetId="1" state="visible" r:id="rId2"/>
@@ -582,11 +582,11 @@
   </sheetPr>
   <dimension ref="A1:Y8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V1" activeCellId="0" sqref="V1:V5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="10.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="34.18"/>
@@ -965,10 +965,10 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="V1:V5 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.73"/>
   </cols>
@@ -1017,10 +1017,10 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="V1:V5 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.98"/>
@@ -1137,10 +1137,10 @@
   <dimension ref="A1:N54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
+      <selection pane="topLeft" activeCell="A28" activeCellId="1" sqref="V1:V5 A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
@@ -2631,10 +2631,10 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="V1:V5 B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.17"/>
@@ -2685,11 +2685,11 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C20" activeCellId="1" sqref="V1:V5 C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.06"/>

</xml_diff>

<commit_message>
change column name gas_temperature to gas_temperature[K] for clarity to users
</commit_message>
<xml_diff>
--- a/tests/edb/data/pointsourceactivities.xlsx
+++ b/tests/edb/data/pointsourceactivities.xlsx
@@ -66,7 +66,7 @@
     <t xml:space="preserve">gas_speed</t>
   </si>
   <si>
-    <t xml:space="preserve">gas_temperature</t>
+    <t xml:space="preserve">gas_temperature[K]</t>
   </si>
   <si>
     <t xml:space="preserve">house_width</t>
@@ -585,11 +585,11 @@
   </sheetPr>
   <dimension ref="A1:Y8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V2" activeCellId="0" sqref="V2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="7.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="34.18"/>
@@ -950,7 +950,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.73"/>
   </cols>
@@ -1002,7 +1002,7 @@
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.98"/>
@@ -1122,7 +1122,7 @@
       <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -2616,7 +2616,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.17"/>
@@ -2671,7 +2671,7 @@
       <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.06"/>

</xml_diff>